<commit_message>
- Documentation - Other missing data for NearZeroCarbon - Adaptation of the get functions for this new scenario
</commit_message>
<xml_diff>
--- a/Inputs/JRC_EU_TIMES/NearZeroCarbon/TIMES_H2_Demand_2050.xlsx
+++ b/Inputs/JRC_EU_TIMES/NearZeroCarbon/TIMES_H2_Demand_2050.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\DispaSET-SideTools\Inputs\JRC_EU_TIMES\NearZeroCarbon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D351A8A9-E9DD-4DFE-9E48-469288002A04}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FEBEEF3-139B-438D-89E9-D7A9853DB147}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="2430" windowWidth="17310" windowHeight="7360" xr2:uid="{F59B6CDE-063C-413C-957A-3E0C28AB0A54}"/>
+    <workbookView xWindow="1060" yWindow="1140" windowWidth="17310" windowHeight="8640" xr2:uid="{E0DE1551-735C-4BD6-A519-86C17B58AEC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,21 +31,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
-  <si>
-    <t>Commodity</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+  <si>
+    <t>Unit - activity1</t>
   </si>
   <si>
     <t>Region</t>
   </si>
   <si>
-    <t>BRFH2</t>
-  </si>
-  <si>
-    <t>INDHH2</t>
-  </si>
-  <si>
-    <t>TRAGH2</t>
+    <t>PJ</t>
   </si>
   <si>
     <t>AT</t>
@@ -109,6 +103,9 @@
   </si>
   <si>
     <t>LV</t>
+  </si>
+  <si>
+    <t>MT</t>
   </si>
   <si>
     <t>NL</t>
@@ -142,9 +139,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.0"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -186,10 +180,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -200,10 +197,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,356 +510,279 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C626C9-D395-43EB-9592-CC2C3A7741FB}">
-  <dimension ref="A1:D32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BD56BA-6490-4D45-9E2B-9A46D3F9308C}">
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B3" s="1">
+        <v>170.51399999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="B4" s="1">
+        <v>449.19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1">
-        <v>110.304</v>
-      </c>
-      <c r="D3" s="1">
-        <v>54.657000000000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="B5" s="1">
+        <v>19.688000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1">
-        <v>90.141999999999996</v>
-      </c>
-      <c r="D4" s="1">
-        <v>100.69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="B6" s="1">
+        <v>38.475999999999992</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1">
-        <v>4.8319999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="B7" s="1">
+        <v>30.782999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1">
-        <v>37.160999999999994</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="B8" s="1">
+        <v>153.482</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="1">
-        <v>1.734</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="B9" s="1">
+        <v>1162.1759999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1">
-        <v>2.4E-2</v>
-      </c>
-      <c r="C8" s="1">
-        <v>77.429000000000002</v>
-      </c>
-      <c r="D8" s="1">
-        <v>75.447000000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+      <c r="B10" s="1">
+        <v>143.18299999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="1">
-        <v>623.07399999999996</v>
-      </c>
-      <c r="D9" s="1">
-        <v>375.69099999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+      <c r="B11" s="1">
+        <v>20.82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="1">
-        <v>1.0529999999999999</v>
-      </c>
-      <c r="D10" s="1">
-        <v>61.29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+      <c r="B12" s="1">
+        <v>154.22800000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="1">
-        <v>9.7119999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
+      <c r="B13" s="1">
+        <v>1152.902</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="1">
-        <v>47.347000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+      <c r="B14" s="1">
+        <v>205.477</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="1">
-        <v>199.369</v>
-      </c>
-      <c r="D13" s="1">
-        <v>599.12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+      <c r="B15" s="1">
+        <v>1919.2190000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="1">
-        <v>59.119</v>
-      </c>
-      <c r="D14" s="1">
-        <v>56.743000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="B16" s="1">
+        <v>15.334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="1">
-        <v>1.006</v>
-      </c>
-      <c r="C15" s="1">
-        <v>174.47900000000001</v>
-      </c>
-      <c r="D15" s="1">
-        <v>567.18899999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+      <c r="B17" s="1">
+        <v>71.384</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="1">
-        <v>2.2669999999999999</v>
-      </c>
-      <c r="D16" s="1">
-        <v>11.98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+      <c r="B18" s="1">
+        <v>20.984000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="1">
-        <v>22.823</v>
-      </c>
-      <c r="D17" s="1">
-        <v>48.561</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+      <c r="B19" s="1">
+        <v>4.3599999999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="1">
-        <v>17.198</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+      <c r="B20" s="1">
+        <v>843.92900000000009</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="1">
-        <v>1.0780000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+      <c r="B21" s="1">
+        <v>7.2620000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="1">
-        <v>310.17700000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
+      <c r="B22" s="1">
+        <v>52.231999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="1">
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
+      <c r="B23" s="1">
+        <v>34.817</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="1">
-        <v>43.923999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
+      <c r="B24" s="1">
+        <v>1.7399999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="1">
-        <v>4.492</v>
-      </c>
-      <c r="D23" s="1">
-        <v>20.675000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
+      <c r="B25" s="1">
+        <v>781.78200000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="1">
-        <v>101.98099999999999</v>
-      </c>
-      <c r="D24" s="1">
-        <v>113.142</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+      <c r="B26" s="1">
+        <v>41.512999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="1">
-        <v>6.99</v>
-      </c>
-      <c r="D25" s="1">
-        <v>11.746</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
+      <c r="B27" s="1">
+        <v>446.18700000000007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="1">
-        <v>2.0179999999999998</v>
-      </c>
-      <c r="C26" s="1">
-        <v>126.464</v>
-      </c>
-      <c r="D26" s="1">
-        <v>298.32100000000003</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+      <c r="B28" s="1">
+        <v>347.87000000000006</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="1">
-        <v>12.145</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
+      <c r="B29" s="1">
+        <v>60.821000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="1">
-        <v>50.851999999999997</v>
-      </c>
-      <c r="D28" s="1">
-        <v>5.5789999999999997</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
+      <c r="B30" s="1">
+        <v>550.62699999999995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="1">
-        <v>10.872</v>
-      </c>
-      <c r="D29" s="1">
-        <v>60.559999999999995</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
+      <c r="B31" s="1">
+        <v>37.045000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="1">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="D30" s="1">
-        <v>33.721000000000004</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="4" t="s">
+      <c r="B32" s="1">
+        <v>106.29600000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="1">
-        <v>0.191</v>
-      </c>
-      <c r="C31" s="1">
-        <v>68.221000000000004</v>
-      </c>
-      <c r="D31" s="1">
-        <v>32.921999999999997</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="1">
-        <v>3.8559999999999999</v>
-      </c>
-      <c r="C32" s="1">
-        <v>126.949</v>
-      </c>
-      <c r="D32" s="1">
-        <v>418.64</v>
+      <c r="B33" s="1">
+        <v>642.64</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:D1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Correct excel files related to H2
</commit_message>
<xml_diff>
--- a/Inputs/JRC_EU_TIMES/NearZeroCarbon/TIMES_H2_Demand_2050.xlsx
+++ b/Inputs/JRC_EU_TIMES/NearZeroCarbon/TIMES_H2_Demand_2050.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\DispaSET-SideTools\Inputs\JRC_EU_TIMES\NearZeroCarbon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FEBEEF3-139B-438D-89E9-D7A9853DB147}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{92D23C93-D3A0-48A4-B4B5-2C14B23B5E39}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1140" windowWidth="17310" windowHeight="8640" xr2:uid="{E0DE1551-735C-4BD6-A519-86C17B58AEC1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E819FEEC-B35E-4799-9FD2-6ED8CCADAD14}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,13 +33,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
-    <t>Unit - activity1</t>
+    <t>Period</t>
   </si>
   <si>
     <t>Region</t>
   </si>
   <si>
-    <t>PJ</t>
+    <t>2050</t>
   </si>
   <si>
     <t>AT</t>
@@ -510,276 +510,278 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BD56BA-6490-4D45-9E2B-9A46D3F9308C}">
-  <dimension ref="A1:B33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F187B333-D8FC-4607-A1D7-FE3DCC71CEF6}">
+  <dimension ref="A2:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B1" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>170.51399999999998</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>449.19</v>
+        <v>165.34299999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>19.688000000000002</v>
+        <v>384.41</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>38.475999999999992</v>
+        <v>7.8729999999999993</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>30.782999999999998</v>
+        <v>37.160999999999994</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>153.482</v>
+        <v>7.7519999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>1162.1759999999999</v>
+        <v>152.876</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>143.18299999999999</v>
+        <v>1078.385</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>20.82</v>
+        <v>82.462999999999994</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>154.22800000000001</v>
+        <v>16.077999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>1152.902</v>
+        <v>131.37700000000001</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>205.477</v>
+        <v>1060.902</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>1919.2190000000001</v>
+        <v>122.435</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>15.334</v>
+        <v>813.42399999999998</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>71.384</v>
+        <v>14.442</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>20.984000000000002</v>
+        <v>71.384</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>4.3599999999999994</v>
+        <v>17.198</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>843.92900000000009</v>
+        <v>3.5739999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>7.2620000000000005</v>
+        <v>403.58500000000004</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>52.231999999999999</v>
+        <v>4.3109999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>34.817</v>
+        <v>43.923999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>1.7399999999999998</v>
+        <v>32.981999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>781.78200000000004</v>
+        <v>1.3879999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>41.512999999999998</v>
+        <v>617.89699999999993</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>446.18700000000007</v>
+        <v>30.905000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>347.87000000000006</v>
+        <v>431.07100000000003</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>60.821000000000005</v>
+        <v>26.777999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>550.62699999999995</v>
+        <v>59.68</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>37.045000000000002</v>
+        <v>128.23699999999999</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>106.29600000000001</v>
+        <v>34.485000000000007</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1">
+        <v>101.143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="1">
-        <v>642.64</v>
+      <c r="B34" s="1">
+        <v>606.94999999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>